<commit_message>
extent report is in progress
</commit_message>
<xml_diff>
--- a/TodoApp/testData/LoginData.xlsx
+++ b/TodoApp/testData/LoginData.xlsx
@@ -66,7 +66,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,19 +76,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -562,155 +549,154 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1042,20 +1028,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="37.2272727272727" customWidth="1"/>
     <col min="2" max="2" width="17.3090909090909" customWidth="1"/>
     <col min="3" max="3" width="18.1545454545455" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" spans="1:4">
+    <row r="1" ht="21" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1065,61 +1051,50 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
     </row>
-    <row r="2" ht="21" spans="1:4">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="21" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2"/>
     </row>
-    <row r="3" ht="21" spans="1:4">
-      <c r="A3" s="3" t="s">
+    <row r="3" ht="21" spans="1:3">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
     </row>
-    <row r="4" ht="21" spans="1:4">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="21" spans="1:3">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2"/>
     </row>
-    <row r="5" ht="21" spans="1:4">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="21" spans="1:3">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>